<commit_message>
Add DateTime to ExtendedPrimitiveTypes, Enum-types render in dynamic panel by default
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelEnumerableRenderTest/TestRenderEmptyEnumerable.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelEnumerableRenderTest/TestRenderEmptyEnumerable.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <x:si>
+    <x:t>Sex</x:t>
+  </x:si>
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -31,8 +34,8 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="3">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="yyyy-MM-dd"/>
-    <x:numFmt numFmtId="166" formatCode="#,0.00"/>
+    <x:numFmt numFmtId="165" formatCode="#,0.00"/>
+    <x:numFmt numFmtId="166" formatCode="yyyy-MM-dd"/>
   </x:numFmts>
   <x:fonts count="1">
     <x:font>
@@ -389,13 +392,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H4"/>
+  <x:dimension ref="A1:K4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:8">
+    <x:row r="2" spans="1:11">
       <x:c r="B2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -405,12 +408,15 @@
       <x:c r="D2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="C3" s="2" t="n">
+    <x:row r="3" spans="1:11">
+      <x:c r="D3" s="1" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="s"/>
+      <x:c r="E3" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>